<commit_message>
evals on full question set
</commit_message>
<xml_diff>
--- a/datasets/itpeu_spd/questions/ITPEU_SPD_Questions.xlsx
+++ b/datasets/itpeu_spd/questions/ITPEU_SPD_Questions.xlsx
@@ -1,31 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\LLamaIndexRAG\questions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sujanrachuri/Desktop/Senior Year/Projects/Sharad/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62E3DDF1-02FB-4D46-8563-0B3600ACABCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{463EDA06-FBBB-914F-89FA-10605F2D5709}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1032" yWindow="840" windowWidth="21948" windowHeight="11232" xr2:uid="{010C08A0-6C74-6440-9812-9E9C7881924C}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="28800" windowHeight="16080" xr2:uid="{010C08A0-6C74-6440-9812-9E9C7881924C}"/>
   </bookViews>
   <sheets>
-    <sheet name="final" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="93">
   <si>
     <t>query</t>
   </si>
@@ -88,13 +99,335 @@
   </si>
   <si>
     <t>If your work schedule is reduced in a way that lowers your Benefit Classification Level under the ITPEU Health and Welfare Plan (for example, from Level IV to Level III due to a decrease from 35 to 25 hours per week), you and your covered family members have the option, at your own expense, to maintain your medical, vision, dental, and prescription drug benefits at the level you had before the change in your work hours. This allows you to continue receiving the same level of benefits despite the reduction in hours, provided you pay the necessary contributions to maintain that level of coverage​.</t>
+  </si>
+  <si>
+    <t>ITPEU_SPD_007</t>
+  </si>
+  <si>
+    <t>ITPEU_SPD_008</t>
+  </si>
+  <si>
+    <t>ITPEU_SPD_009</t>
+  </si>
+  <si>
+    <t>ITPEU_SPD_010</t>
+  </si>
+  <si>
+    <t>ITPEU_SPD_011</t>
+  </si>
+  <si>
+    <t>My contribution rate is $3.35/hr and I work a regular 40 hrs/week. What do I have to pay for when I visit the doctor?</t>
+  </si>
+  <si>
+    <t>What does my plan cover for dental and prescription drugs?</t>
+  </si>
+  <si>
+    <t>Dental Benefits:
+Deductible: You are responsible for paying a deductible amount per calendar year for dental expenses.
+Coverage: After the deductible, the plan pays 75% of the balance of any covered dental expense, except for prosthetics and teeth cleaning.
+Prosthetics: The plan pays 45% of charges related to prosthetics after you have been continually eligible for benefits for twelve (12) consecutive months, up to the maximum dental benefit. You are entitled to benefits for one prosthetic appliance in any period of five (5) consecutive years.
+Teeth Cleaning: Dental benefits for teeth cleaning are covered in the same manner as other dental benefits and are limited to one treatment in any period of six (6) consecutive months.
+Exclusions: There are specific exclusions which are not covered, including services incurred before eligibility, charges related to congenital malformations unless after 36 consecutive months of eligibility, treatments for cosmetic purposes, and charges for orthodontic services.
+Prescription Drug Benefits:
+Coverage: The plan covers 75% of the charge for prescription drugs, up to the maximum benefit specified in the Schedule of Benefits.
+Prescription Drug: Defined as a drug available to the public only upon prescription written by a licensed Physician or Health Care Provider.
+Prescription: A written order for dispensing and administering drugs signed by a Physician or licensed Health Care Provider.
+Birth Control: Benefits for prescription birth control are payable to female Employees or wives of male Employees.
+Exclusions: Certain medications and scenarios are excluded from coverage, such as medications withdrawn from the market, non-prescription drugs, and drugs used for cosmetic purposes.
+To understand the exact deductible amounts, coverage limits, and any copays for specific dental procedures and prescription drugs, you should refer to your Schedule of Benefits. This document will detail the exact financial responsibilities based on your contribution rate and class level, as well as the specifics of the coverage for dental and prescription drug benefits.</t>
+  </si>
+  <si>
+    <t>Based on the context provided from your plan document, here are the steps to take for an appeal and the associated timelines:
+Notice of Denial: If your claim is denied, you will receive a written notice with the details of the claim, reasons for denial, plan provisions cited, and any additional material or information required to perfect your claim.
+Filing an Appeal: You have the right to appeal an adverse benefit determination. You must file your appeal within 180 calendar days after receiving the denial notice.
+Supporting Information: You can submit written comments, documents, records, and any other information you believe supports your claim.
+Review Process: The Claims Administrator will review all submitted information, regardless of whether it was considered in the initial decision.
+Independent Reviewer: The appeal will be conducted by an individual who is not subordinate to any person who made the initial decision, and who did not participate in the initial decision if the denial was based in whole or part on medical judgment.
+Timeline for a Decision:
+For pre-service claims (claims for benefits that require approval before receiving medical care): The plan will provide a decision within a reasonable time appropriate to the medical circumstances but no later than 30 days after receipt of the appeal.
+For post-service claims (claims for benefits after services are provided): The plan will provide a decision on the appeal no later than 60 days after receipt of the appeal.
+Urgent Care Claims: Expedited appeal procedures are available for claims involving urgent care. The Claims Administrator must notify you of their decision as soon as possible, considering medical exigencies, but no later than 72 hours after receipt of the appeal.
+External Review: If your internal appeal is not resolved in your favor, you can request an independent external review within four (4) months of the notice of the final internal adverse determination.
+Expedited External Review: This can be requested for urgent care claims without completing the internal appeal process or while simultaneously pursuing an expedited internal appeal.
+Final Decision: The Claims Administrator will notify you of the final decision after the internal appeal process and provide the rationale if the decision is adverse.
+Timeline for External Review: For non-urgent care claims, the external review decision must be provided no later than 45 days after the external review is requested.
+Legal Action: If your appeal results in an adverse benefit determination, you have the right to bring a civil action under Section 502(a) of ERISA.
+Requirement to Appeal Before Lawsuit: You must complete the internal appeal process before you can file a lawsuit regarding the benefit decision.</t>
+  </si>
+  <si>
+    <t>If you visit the doctor, as a participant with a contribution rate of $3.35 per hour, you fall below the special rule threshold for participants in Class III and IV, which is set at a contribution rate of $3.75 per hour or higher. Therefore, the special co-pay rule does not apply to you. Here's what you'd generally be responsible for:
+Deductible: You'll be responsible for paying a deductible each calendar year. This deductible applies regardless of the number of injuries or illnesses you may have.
+Family Maximum Deductibles: If applicable, there is a maximum of two deductibles per family per calendar year.
+Coverage for In-Network Expenses: After you've paid your deductible, the Fund will cover 70% of all covered medical expenses within the network, up to your Out Of Pocket Maximum or the annual Maximum Medical Benefit specified in the Schedule of Benefits. Once you've reached your Out Of Pocket Maximum and if you haven't reached your annual Maximum Medical Benefit, the Fund will cover 100% of the additional covered medical expenses.
+Coverage for Out-of-Network Expenses: For services out of the network, after your deductible, the Fund will cover 60% of all covered medical expenses, following the same rules regarding the Out Of Pocket Maximum and the Maximum Medical Benefit.
+Participant's Responsibility: Aside from the deductible, you are responsible for paying 30% of In-Network covered medical expenses and 40% of Out-of-Network covered medical expenses, up until you reach your Out Of Pocket Maximum. Any expenses beyond the Maximum Medical Benefit for the year are your responsibility.
+Maximum Medical Benefit: This is the total amount the Fund will pay for your covered medical expenses, both In and Out of Network, per calendar year. It includes all benefits paid at 60%, 70%, and 100% rates.
+Since your contribution rate is $3.35/hr, for any doctor visit, you'd need to pay the deductible first. After that, for in-network services, you'd be responsible for 30% of the remaining costs until you reach your Out Of Pocket Maximum, at which point the plan would cover at 100% up to the Maximum Medical Benefit for the year. For out-of-network services, you would be responsible for 40% of the costs post-deductible until reaching the Out Of Pocket Maximum. The exact amounts for your deductible, Out Of Pocket Maximum, and Maximum Medical Benefit would be specified in your Schedule of Benefits, which should be referenced for detailed figures.</t>
+  </si>
+  <si>
+    <t>What is required to apply for continuation of coverage and how long does it last and cost?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To apply for continuation of coverage under your plan:
+Requirements to Apply:
+Enrollment Card Submission: An employee or covered family member must have submitted an enrollment card to the Fund Office with full names and addresses.
+Qualifying Event: You must experience a Qualifying Event, such as termination of employment, death of the employee, divorce or legal separation, loss of covered child status, reduction in weekly work schedule, or exhaustion of leave under FMLA without a return to employment.
+Notification: You must notify the Fund Office of the Qualifying Event. Employers are required to notify within 30 days if it relates to death, termination, or reduction in hours. For divorce, legal separation, or loss of covered child status, the employee or covered family member has 60 days to notify.
+Election of Coverage: You have 60 days to elect continuation of coverage after the later of the date you would lose coverage or the date you are sent notice by the Fund Office.
+Duration of Coverage:
+Termination or Reduction in Hours: Maximum of 18 months from the date of the Qualifying Event.
+Death, Divorce, Separation, or Loss of Child Status: Maximum of 36 months.
+Extended Duration: If a second Qualifying Event occurs, the 18-month period may extend to 36 months from the date of the first Qualifying Event.
+Disability Extension: If you are determined by the SSA to have been disabled at the time of the Qualifying Event, the 18-month period may extend to 29 months.
+Cost of Coverage:
+Premium Calculation: The premium is 102% of the cost calculated by the Trustees and Fund actuary. You will be notified of the amount in the notice following the Qualifying Event.
+Premium Adjustments: Premiums are established yearly on October 1. Any increase during a coverage period will be notified by October 15th, and the new premium must be paid to continue coverage.
+Payment Timeliness: Premium payments must be made no later than 30 days following the month they are due.
+Coverage Upon Late Election: If the election is made after the Qualifying Event, coverage is provided retrospectively as long as the first premium payment is made within 45 days of the election.
+Failure to Pay: If premiums are not timely paid, eligibility for continuation of coverage ceases.
+Special Provisions: Between September 1, 2008, and May 31, 2010, those involuntarily terminated may have been eligible for a 65% premium reduction for up to 9 months, governed by the ARRA.
+Remember, the specific costs will depend on the premiums set for the coverage year and can change annually. If you need more detailed information about the cost, you would need to contact the Fund Office or refer to the additional documentation provided by the plan.
+</t>
+  </si>
+  <si>
+    <t>I recently gave birth to a child and am on my 11th week of maternity leave. I want to take leave for some more time, how do I stay covered?</t>
+  </si>
+  <si>
+    <t>Since you are currently on your 11th week of maternity leave and you want to extend your leave, here's how you can stay covered:
+FMLA Leave: You have been utilizing the Family and Medical Leave Act (FMLA) leave, which entitles eligible employees to up to 12 weeks of unpaid leave for the birth and care of a child. Since you're in the 11th week, you have 1 more week of FMLA leave available.
+Extension of Benefits: After exhausting the 12 weeks provided by FMLA, you are entitled to an extension of benefits from your Plan for a period of two months from the date of your last contribution period. This extension is in addition to the FMLA leave, provided specifically for your own disability related to childbirth.
+Application for Continuation: You do not need to apply for Continuation of Coverage under Section 15 of your Plan during the FMLA leave and the subsequent two-month extension.
+After FMLA and Extension: Once you have exhausted both the FMLA leave and the two-month extension, if you wish to continue your leave and maintain health coverage, you will need to apply for Continuation of Coverage as outlined in Section 15 of the Plan.
+In summary, after your FMLA leave ends following the 12th week, you can extend your health benefits for an additional two months as part of the plan's provision. Should you need more time beyond this, you would apply for Continuation of Coverage according to the guidelines of your plan.</t>
+  </si>
+  <si>
+    <t>ITPEU_SPD_012</t>
+  </si>
+  <si>
+    <t>ITPEU_SPD_013</t>
+  </si>
+  <si>
+    <t>ITPEU_SPD_014</t>
+  </si>
+  <si>
+    <t>ITPEU_SPD_015</t>
+  </si>
+  <si>
+    <t>ITPEU_SPD_016</t>
+  </si>
+  <si>
+    <t>ITPEU_SPD_017</t>
+  </si>
+  <si>
+    <t>ITPEU_SPD_018</t>
+  </si>
+  <si>
+    <t>ITPEU_SPD_019</t>
+  </si>
+  <si>
+    <t>ITPEU_SPD_020</t>
+  </si>
+  <si>
+    <t>ITPEU_SPD_021</t>
+  </si>
+  <si>
+    <t>ITPEU_SPD_022</t>
+  </si>
+  <si>
+    <t>ITPEU_SPD_023</t>
+  </si>
+  <si>
+    <t>ITPEU_SPD_024</t>
+  </si>
+  <si>
+    <t>ITPEU_SPD_025</t>
+  </si>
+  <si>
+    <t>I am a recent hire. My spouse and I aren't legally separated, but we have been living apart for a year. Is she covered?</t>
+  </si>
+  <si>
+    <t>Based on the document you provided, your spouse would not be considered a covered family member under your health plan if you have been living apart for a year or more. The document states:
+"A. The Spouse of an Employee provided that a person shall not be considered a Spouse of an Employee if that person is either divorced from the Employee, legally separated from the Employee or has not resided with the Employee for one year or more prior to the date any benefit specified in this Plan becomes due."
+Given this condition, your spouse would not be eligible for coverage under the current terms of the plan as described. If you have additional questions or need further clarification on your benefits, you may want to consult your plan administrator directly.</t>
+  </si>
+  <si>
+    <t>How do I go about listing a beneficiary?</t>
+  </si>
+  <si>
+    <t>To list a beneficiary for your plan, the document outlines a specific process that you should follow:
+Form of Designation of Beneficiary: Your designation of a beneficiary must be in writing on a form supplied for this purpose by the Trustees. It's important that you use the official form to ensure that your designation is valid.
+Filing the Form: Once you have completed the beneficiary designation form, it must be on file at the principal office of the Fund to be considered valid.
+Change of Beneficiary: If you wish to change your beneficiary in the future, you can do so by completing and filing a new beneficiary form at the principal office of the Fund. This new designation will replace any previous designations.
+Here's what you might consider doing next:
+Contact the plan administrator or visit the office where your plan is managed to request a beneficiary designation form.
+Fill out the form as instructed, clearly indicating the beneficiary or beneficiaries you wish to designate.
+Submit the completed form to the required office to ensure it is on file.
+This process will officially record your choice of beneficiary for your plan benefits.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I regularly work 40 hrs/week on average. What type of coverage do I have? </t>
+  </si>
+  <si>
+    <t>Based on your regular work hours of 40 hours per week, you fall into the highest classification for benefit levels according to the document. Here’s how the benefit classifications are set up:
+Classification Levels:
+Level I: Less than 12 hours per week
+Level II: 12 through 19 hours per week
+Level III: 20 through 29 hours per week
+Level IV: 30 hours or more per week
+Since you work 40 hours per week on average, you are classified under Level IV. This level typically provides the highest level of benefits available under the plan. While the document does not specify the exact benefits for each level in the sections provided, Level IV generally includes comprehensive coverage, which may encompass health, dental, vision, and possibly additional benefits like accidental death and dismemberment insurance.
+To understand the specific benefits you are entitled to under Level IV, you would need to look at the detailed Schedule of Benefits provided by your plan. This schedule will outline the specifics of what is covered, including the extent of coverage for medical services, prescriptions, and other health-related expenses.</t>
+  </si>
+  <si>
+    <t>How are death benefits calculated?</t>
+  </si>
+  <si>
+    <t>Death benefits under your plan are calculated and distributed according to several key provisions:
+Employee Death (Section 5.01): If an employee dies from any cause during a period of their eligibility or within 31 days after their eligibility ends, the plan will pay the death benefit amount to the designated beneficiary as specified in the Schedule of Benefits.
+Continuation During Disability (Section 5.02): If an employee becomes totally and permanently disabled while eligible, their death benefit eligibility continues for two years or a period equal to their service with their employer (whichever is less), without further contributions.
+Death of a Covered Family Member (Section 5.03): If a covered family member dies while the employee is eligible for benefits, the employee will receive the full amount specified in the Schedule of Benefits.
+Single Employee’s Additional Benefit (Section 5.04): If an employee who is single dies while eligible for benefits, an additional $1,000.00 is added to the death benefit amount provided in the Schedule of Benefits.
+Non-Occupational Accidental Death and Dismemberment (Section 6): If an employee suffers dismemberment or dies due to a covered accident while eligible, the fund pays benefits as described in Section 6.02, which outlines specific amounts for dismemberment or accidental death, according to the Schedule of Benefits.
+Survivor Death Benefits (Section 7.01): In addition to the death benefits described above, the fund pays a Survivor Death Benefit in monthly installments as outlined in the Schedule of Benefits.
+To determine the exact amount for each of these benefits, you would refer to the Schedule of Benefits. This document will provide specific benefit amounts and further details on the coverage provided under the plan.</t>
+  </si>
+  <si>
+    <t>ITPEU_SPD_026</t>
+  </si>
+  <si>
+    <t>ITPEU_SPD_027</t>
+  </si>
+  <si>
+    <t>ITPEU_SPD_028</t>
+  </si>
+  <si>
+    <t>ITPEU_SPD_029</t>
+  </si>
+  <si>
+    <t>ITPEU_SPD_030</t>
+  </si>
+  <si>
+    <t>Are hearing aids covered?</t>
+  </si>
+  <si>
+    <t>Hearing aids are indeed covered for Employees and their Dependents if the contribution rates are $3.24 per hour and above. The Schedule of Benefits determines the exact dollar amount for each hearing aid benefit payable by the Fund. The coverage is subject to the following conditions:
+The maximum amount that the Fund will pay for any Employee or Dependent is fixed and will not exceed the specified limit in any 24-month period.
+The medical benefits under which hearing aids are covered renew each calendar year, but this does not include hearing aid benefits, which are governed by their own specific provisions as outlined in the plan document.
+For the exact coverage details, such as the maximum dollar amount and any specific exclusions or limitations that apply to hearing aid benefits, you should refer directly to the Schedule of Benefits in your plan documents or contact your plan administrator for clarification.</t>
+  </si>
+  <si>
+    <t>How can I contact the claims administrator?</t>
+  </si>
+  <si>
+    <t>You can contact the Claims Administrator by calling 1-877-331-4329. This number should connect you with a representative who can assist you with any questions about your plan.</t>
+  </si>
+  <si>
+    <t>Is breastfeeding covered?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Breastfeeding support, supplies, and counseling are indeed covered by the plan. The coverage is part of the Women's Health Care preventive services that are paid at 100% by the plan when provided by Network Healthcare Providers, in compliance with the Affordable Care Act. This typically includes the provision of breast pumps (limited to one per calendar year), which is an essential aspect of breastfeeding support.
+</t>
+  </si>
+  <si>
+    <t>Are sunglasses covered?</t>
+  </si>
+  <si>
+    <t>The plan specifically excludes coverage for sunglasses, whether they are plain or prescription. According to Section 11.04, restrictions on the payment of vision benefits, item (d), the vision care benefits do not cover sunglasses or safety lenses or goggles.</t>
+  </si>
+  <si>
+    <t>Are nova pens covered?</t>
+  </si>
+  <si>
+    <t>Based on the exclusions listed in Section 23 of your plan, nova pens, which are typically used for the administration of insulin, are specifically excluded from coverage. Item 15 under the exclusions states that "blood/injection related items: blood pressure cuffs, centrifuges, nova pens, needle-less injectors" are not covered. This means that if you require a nova pen for diabetes management, you would need to seek alternative coverage options or discuss other possible solutions with your healthcare provider or the Claims Administrator.</t>
+  </si>
+  <si>
+    <t>My wife and I are both employees. How are our benefits distributed?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+If both a husband and wife are employees, benefits for each are used first from their own employment. Once those are exhausted, they can then access benefits available through their status as a Covered Family Member of their spouse. The plan ensures that the total benefits do not exceed the maximum allowed for the claim.
+For any children covered by the plan, additional provisions determine how their benefits are distributed, taking into account factors such as the length of employment of each parent. These rules are designed to coordinate coverage without surpassing the plan's maximum benefit limit for any claims.</t>
+  </si>
+  <si>
+    <t>My divorced spouse is covered by another plan and both of our plans cover our child. How are our benefits distributed?</t>
+  </si>
+  <si>
+    <t>When both divorced parents have plans that cover their child, the benefits for the child are coordinated in a specific order, as outlined in your plan document:
+Plan of the parent obligated by a Qualified Medical Support Order: If one parent is required by such an order to provide health benefits, that parent's plan pays first.
+Plan of the parent with whom the child primarily resides: Benefits from this plan are used second.
+Plan of the spouse of the parent with whom the child primarily resides: This plan pays next.
+Plan of the parent with whom the child does not reside: This plan pays last.</t>
+  </si>
+  <si>
+    <t>What coverage is provided for braces?</t>
+  </si>
+  <si>
+    <t>Coverage for braces is specifically excluded from your plan's covered dental expenses. Orthodontic services, including braces, are not covered under the provided benefits​.</t>
+  </si>
+  <si>
+    <t>In your situation, if you're unable to work due to sickness, your claim for weekly accident and sickness benefit would be considered "incurred" on the fourth day of your disability as brought about by illness. This is when your eligibility to file a claim would begin, according to the plan document. So you should submit your claim for the sickness benefits after the fourth day of your disability. Remember, you have one year from this "incurred" date to file the claim​​.</t>
+  </si>
+  <si>
+    <t>I need to get an organ transplant. How do I ensure I stay covered and how much leave can I qualify for?</t>
+  </si>
+  <si>
+    <t>To ensure you remain covered for an organ transplant, you need to follow the pre-certification requirements set forth by your plan. All transplant procedures must be pre-certified to confirm they are medically appropriate based on criteria established by the plan. This means you should work with your healthcare provider to get the necessary approval from your plan before proceeding with the transplant .
+As for leave, if you're unable to work due to your medical condition, you might qualify for leave under the Family and Medical Leave Act (FMLA). Eligible employees are entitled to up to 12 workweeks of unpaid leave in a 12-month period for serious health conditions that make them unable to perform their job. Additionally, if you are undergoing treatment for your own disability, you might be entitled to an extension of benefits from the plan for a period of two months from the date of your last contribution period after utilizing any period of leave covered by the FMLA .
+To maintain coverage during your leave, you might be able to make self-payments to continue your benefits. This is sometimes referred to as COBRA continuation coverage, which allows you to keep your group health insurance coverage under certain circumstances such as job loss or reduction in hours worked, among others .
+If your situation is urgent and requires immediate attention, the plan provides for expedited appeal processes for urgent care claims, which would be relevant if you're dealing with an immediate need for a transplant and associated services .</t>
+  </si>
+  <si>
+    <t>How do I know if I'm responsible for getting pre-certification and how long does it take?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You're responsible for obtaining pre-certification if services are provided by a network provider outside of certain states (California, Colorado, Connecticut, Georgia, Indiana, Kentucky, Maine, Missouri, New Hampshire, Nevada, Ohio, Virginia, and Wisconsin) or by any out-of-network healthcare provider. In these scenarios, you or your authorized representative must ensure that pre-certification has been obtained.
+For non-urgent pre-certification requests, the claims administrator typically responds within 15 calendar days of receiving the request. If the pre-certification request is urgent, the claims administrator should respond within 72 hours.
+In the event of an emergency admission to a hospital, you or your representative must notify the claims administrator within two business days after the admission, or as soon as reasonably possible, to adhere to the plan’s requirements and maintain coverage for the services provided​​.
+</t>
+  </si>
+  <si>
+    <t>I recently tried to file a medical benefits claim and it was denied. What steps do I take for an appeal and how long will it take?</t>
+  </si>
+  <si>
+    <t>My daughter recently had a child. Does the plan cover her maternity care?</t>
+  </si>
+  <si>
+    <t>Maternity care is treated as any other illness under the plan for female employees or wives of employees, meaning it is a covered benefit. However, no benefits will be paid by the Fund for any medical treatment arising out of maternity care for covered children of employees . If your daughter is a dependent covered under your plan, her maternity care would not be covered by the plan based on this provision.</t>
+  </si>
+  <si>
+    <t>I have a family of 4 covered by my plan. How many deductibles need to be paid for?</t>
+  </si>
+  <si>
+    <t>For your health plan, as it covers your family of four, the deductible structure is as follows:
+Medical Benefits: There is a deductible for each participant, but the plan specifies a maximum of two deductibles per family per calendar year. This means regardless of how many family members incur medical expenses, only two deductibles need to be paid in total for the family each year.
+Dental Benefits: Each person covered by the plan must pay the deductible for dental expenses each calendar year. This implies that each family member would be responsible for their own dental deductible.
+Therefore, for medical expenses, your family would pay up to two deductibles in total for the year, regardless of how many of you incur expenses. For dental expenses, each family member would need to meet their individual deductible.</t>
+  </si>
+  <si>
+    <t>Can I get my daughter's birth control covered?</t>
+  </si>
+  <si>
+    <t>Yes, the plan covers birth control, but it is specifically limited to female employees or the wives of male employees. Here's the relevant excerpt from the plan document regarding prescription drug benefits:
+Section 13.04 Birth Control: Birth control benefits shall be payable only to female employees or wives of male employees.
+This means that if your daughter is a covered family member under your plan and not an employee herself, she would not be eligible for birth control benefits under this provision. The benefit is designed to apply only to women who are either employees themselves or the spouses of male employees within the plan.</t>
+  </si>
+  <si>
+    <t>I recently got seriously sick and can't work. How soon can I make a claim?</t>
+  </si>
+  <si>
+    <t>I recently got eye surgery and now need vision therapy treatment. Is this covered?</t>
+  </si>
+  <si>
+    <t>Based on the information provided in Section 23, General Exclusions and Limitations of the plan document, particularly item 13, vision therapy is covered only if it's needed due to intraocular surgery. Here's the specific clause:
+Item 13: Vision therapy unless needed due to intraocular surgery.
+If your eye surgery was intraocular (pertaining to or occurring within the eye), and the vision therapy treatment is considered necessary as part of your recovery from that surgery, then it would be covered according to the plan. However, if the surgery was not intraocular or if the therapy is not directly related to recovery from intraocular surgery, it would not be covered under this plan.
+It's important to have your physician or surgeon confirm that the vision therapy is indeed necessary post-intraocular surgery to ensure coverage according to these plan terms.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -172,9 +505,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -212,7 +545,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -318,7 +651,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -460,7 +793,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -468,20 +801,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7929DB3-7C5A-3945-A750-F8690354D5ED}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="75" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.19921875" customWidth="1"/>
-    <col min="2" max="2" width="55.296875" customWidth="1"/>
-    <col min="3" max="3" width="39" customWidth="1"/>
+    <col min="1" max="1" width="22.1640625" customWidth="1"/>
+    <col min="2" max="2" width="55.33203125" customWidth="1"/>
+    <col min="3" max="3" width="130.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -492,8 +825,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="240.6">
-      <c r="A2" t="s">
+    <row r="2" spans="1:3" ht="85" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
@@ -503,8 +836,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="210.6">
-      <c r="A3" t="s">
+    <row r="3" spans="1:3" ht="68" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
@@ -514,8 +847,8 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="150.6">
-      <c r="A4" t="s">
+    <row r="4" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="s">
@@ -525,7 +858,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="135.6">
+    <row r="5" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
@@ -536,7 +869,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="240.6">
+    <row r="6" spans="1:3" ht="68" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
@@ -547,7 +880,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="120.6">
+    <row r="7" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
@@ -558,10 +891,269 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="4"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="1"/>
+    <row r="8" spans="1:3" ht="409.5" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="409.5" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="409.5" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="409.5" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="289" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="153" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="221" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="255" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="289" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="136" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="153" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="68" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="119" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="136" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="68" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="255" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="272" x14ac:dyDescent="0.2">
+      <c r="A27" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A28" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="136" x14ac:dyDescent="0.2">
+      <c r="A29" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="119" x14ac:dyDescent="0.2">
+      <c r="A30" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="170" x14ac:dyDescent="0.2">
+      <c r="A31" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>92</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>